<commit_message>
Assigned achievements to everyone
See the issue post for more info
</commit_message>
<xml_diff>
--- a/heights.xlsx
+++ b/heights.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Documents\GitHub\CommonSquirrel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zachary\Documents\GitHub\CommonSquirrel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>Tree Sapling</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t xml:space="preserve">Squilnit the Soviet Squirrel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">will </t>
+  </si>
+  <si>
+    <t xml:space="preserve">zach </t>
+  </si>
+  <si>
+    <t xml:space="preserve">steven </t>
   </si>
 </sst>
 </file>
@@ -540,21 +549,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,8 +576,11 @@
       <c r="D1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -578,8 +590,11 @@
       <c r="D2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -592,8 +607,11 @@
       <c r="D3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -606,8 +624,11 @@
       <c r="D4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -617,8 +638,11 @@
       <c r="D5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -628,8 +652,11 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -639,8 +666,11 @@
       <c r="D7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -650,8 +680,11 @@
       <c r="D8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -661,8 +694,11 @@
       <c r="D9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -672,8 +708,11 @@
       <c r="D10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -683,8 +722,11 @@
       <c r="D11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -694,8 +736,11 @@
       <c r="D12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -705,8 +750,11 @@
       <c r="D13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -716,8 +764,11 @@
       <c r="D14" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -727,8 +778,11 @@
       <c r="D15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -738,8 +792,11 @@
       <c r="D16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -749,8 +806,11 @@
       <c r="D17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -760,8 +820,11 @@
       <c r="D18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -771,8 +834,11 @@
       <c r="D19" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -782,8 +848,11 @@
       <c r="D20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -793,8 +862,11 @@
       <c r="D21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -804,8 +876,11 @@
       <c r="D22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -815,8 +890,11 @@
       <c r="D23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -826,8 +904,11 @@
       <c r="D24" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -837,8 +918,11 @@
       <c r="D25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -848,8 +932,11 @@
       <c r="D26" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -862,8 +949,11 @@
       <c r="D27" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -876,8 +966,11 @@
       <c r="D28" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -890,8 +983,11 @@
       <c r="D29" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -903,6 +999,9 @@
       </c>
       <c r="D30" t="s">
         <v>54</v>
+      </c>
+      <c r="E30" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>